<commit_message>
Added SVM RBF Calibration
</commit_message>
<xml_diff>
--- a/report/KernelSVM.xlsx
+++ b/report/KernelSVM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Giorgio/Lavoro/Polito_Magistrale/MACHINE_LEARNING_PATTER_REC/Esame/wine-quality-detection/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848BB5A2-25E6-F045-A389-F4E3F131FB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4AD345-4441-B744-B6C4-091B6E4F891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="500" windowWidth="35840" windowHeight="20760" xr2:uid="{DF034D36-0A02-1048-85AB-CA17B5DC662C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" xr2:uid="{DF034D36-0A02-1048-85AB-CA17B5DC662C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>LogReg ( l = 1e-5, ptrain = 0.1)</t>
   </si>
@@ -150,9 +150,6 @@
     <t>d=2</t>
   </si>
   <si>
-    <t>Gaussiana</t>
-  </si>
-  <si>
     <t>0.704</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>0.630</t>
   </si>
   <si>
-    <t>C Migliore = 1</t>
-  </si>
-  <si>
     <t>MIN DCF / ACTUAL DCF</t>
   </si>
   <si>
@@ -223,6 +217,45 @@
   </si>
   <si>
     <t>0.242</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.715</t>
+  </si>
+  <si>
+    <t>0.267</t>
+  </si>
+  <si>
+    <t>0.768</t>
+  </si>
+  <si>
+    <t>0.272</t>
+  </si>
+  <si>
+    <t>0.726</t>
+  </si>
+  <si>
+    <t>0.663</t>
+  </si>
+  <si>
+    <t>0.291</t>
+  </si>
+  <si>
+    <t>0.852</t>
+  </si>
+  <si>
+    <t>0.778</t>
+  </si>
+  <si>
+    <t>0.487</t>
   </si>
 </sst>
 </file>
@@ -232,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +311,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,6 +450,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -724,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADFF9A9-63F9-D646-97F5-374C7C9483F9}">
-  <dimension ref="A3:T45"/>
+  <dimension ref="A3:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="137" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,7 +787,10 @@
     <col min="8" max="8" width="5.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="15" style="2" customWidth="1"/>
-    <col min="11" max="19" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="12.33203125" style="2" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="2"/>
+    <col min="15" max="15" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.83203125" style="2"/>
     <col min="20" max="20" width="39.1640625" style="2" customWidth="1"/>
     <col min="21" max="23" width="10.83203125" style="2"/>
     <col min="24" max="24" width="34.1640625" style="2" customWidth="1"/>
@@ -767,11 +815,11 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="I6" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
@@ -796,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -807,7 +855,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="I9" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K9"/>
       <c r="L9"/>
@@ -827,7 +875,7 @@
         <v>12</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>10</v>
@@ -853,7 +901,7 @@
         <v>30</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>25</v>
@@ -893,21 +941,21 @@
         <v>33</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -918,16 +966,16 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="I15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="L15" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
@@ -1003,7 +1051,6 @@
     <row r="24" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D24" s="3"/>
       <c r="I24" s="1"/>
-      <c r="N24" s="1"/>
     </row>
     <row r="25" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
@@ -1026,14 +1073,6 @@
       <c r="F26" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I27" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="28" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
@@ -1048,13 +1087,13 @@
         <v>17</v>
       </c>
       <c r="D29" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="F29" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
@@ -1065,10 +1104,10 @@
         <v>13</v>
       </c>
       <c r="E30" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
@@ -1076,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="F31" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1090,44 +1129,124 @@
         <v>1</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="16"/>
-    </row>
-    <row r="42" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
+    <row r="35" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B37"/>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="30"/>
+    </row>
+    <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39" s="19"/>
+      <c r="K39" s="29"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="O40" s="30"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="31"/>
+    </row>
+    <row r="42" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>